<commit_message>
adding info to olld experiments
</commit_message>
<xml_diff>
--- a/PrepSheet_Autofill_Template_Update032520.xlsx
+++ b/PrepSheet_Autofill_Template_Update032520.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033767D1-1EB8-A34A-A4BB-A5FACDA66975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44B6F80-969D-7849-AA8F-AA10ECC36927}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7400" yWindow="5460" windowWidth="17640" windowHeight="18940" firstSheet="6" activeTab="11" xr2:uid="{87223161-21E3-D547-BEAF-2AFC325C2C31}"/>
+    <workbookView xWindow="7400" yWindow="460" windowWidth="17640" windowHeight="18940" activeTab="6" xr2:uid="{87223161-21E3-D547-BEAF-2AFC325C2C31}"/>
   </bookViews>
   <sheets>
     <sheet name="Objs.Directions" sheetId="17" r:id="rId1"/>
@@ -9149,7 +9149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4958B5-37FB-2944-8284-DDBDEBA5917C}">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -23515,8 +23515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB832963-2F29-F34D-9B52-048A446EDD8F}">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J41"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26059,7 +26059,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I41" xr:uid="{D5AB58AB-ED89-9E43-8573-41B3B561C60B}">
       <formula1>"E7420L"</formula1>
     </dataValidation>
@@ -26069,8 +26069,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H41" xr:uid="{F346031A-CF56-2C45-9868-80810296170D}">
       <formula1>"E7490L"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J41" xr:uid="{5AF46E1E-D4D0-4C4D-A9CA-84AC40AD5910}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J41" xr:uid="{5AF46E1E-D4D0-4C4D-A9CA-84AC40AD5910}">
       <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{3C4F6157-34ED-3D47-9E58-1553D6024B06}">
+      <formula1>"True, False"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed to conform to standard
</commit_message>
<xml_diff>
--- a/PrepSheet_Autofill_Template_Update032520.xlsx
+++ b/PrepSheet_Autofill_Template_Update032520.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44B6F80-969D-7849-AA8F-AA10ECC36927}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136F2408-1734-FE40-9C26-99B66D0E4D93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7400" yWindow="460" windowWidth="17640" windowHeight="18940" activeTab="6" xr2:uid="{87223161-21E3-D547-BEAF-2AFC325C2C31}"/>
   </bookViews>
@@ -35,18 +35,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="510">
   <si>
     <t>Genomic #</t>
   </si>
@@ -1573,6 +1567,9 @@
   </si>
   <si>
     <t>PoolledSecondStrand</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -1867,7 +1864,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2091,6 +2088,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -23515,7 +23513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB832963-2F29-F34D-9B52-048A446EDD8F}">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -23587,8 +23585,8 @@
       <c r="I2" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J2" s="21" t="b">
-        <v>0</v>
+      <c r="J2" s="129" t="s">
+        <v>509</v>
       </c>
       <c r="K2" s="21" t="s">
         <v>361</v>
@@ -23626,7 +23624,7 @@
       <c r="I3" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J3" s="21" t="b">
+      <c r="J3" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K3" s="21" t="s">
@@ -23665,7 +23663,7 @@
       <c r="I4" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J4" s="21" t="b">
+      <c r="J4" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K4" s="21" t="s">
@@ -23704,7 +23702,7 @@
       <c r="I5" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J5" s="21" t="b">
+      <c r="J5" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K5" s="21" t="s">
@@ -23743,7 +23741,7 @@
       <c r="I6" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J6" s="21" t="b">
+      <c r="J6" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K6" s="21" t="s">
@@ -23782,7 +23780,7 @@
       <c r="I7" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J7" s="21" t="b">
+      <c r="J7" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K7" s="21" t="s">
@@ -23821,7 +23819,7 @@
       <c r="I8" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J8" s="21" t="b">
+      <c r="J8" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K8" s="21" t="s">
@@ -23860,7 +23858,7 @@
       <c r="I9" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J9" s="21" t="b">
+      <c r="J9" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K9" s="21" t="s">
@@ -23899,7 +23897,7 @@
       <c r="I10" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J10" s="21" t="b">
+      <c r="J10" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K10" s="21" t="s">
@@ -23938,7 +23936,7 @@
       <c r="I11" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J11" s="21" t="b">
+      <c r="J11" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K11" s="21" t="s">
@@ -23977,7 +23975,7 @@
       <c r="I12" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J12" s="21" t="b">
+      <c r="J12" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K12" s="21" t="s">
@@ -24016,7 +24014,7 @@
       <c r="I13" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J13" s="21" t="b">
+      <c r="J13" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K13" s="21" t="s">
@@ -24055,7 +24053,7 @@
       <c r="I14" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J14" s="21" t="b">
+      <c r="J14" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K14" s="21" t="s">
@@ -24094,7 +24092,7 @@
       <c r="I15" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J15" s="21" t="b">
+      <c r="J15" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K15" s="21" t="s">
@@ -24133,7 +24131,7 @@
       <c r="I16" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J16" s="21" t="b">
+      <c r="J16" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K16" s="21" t="s">
@@ -24172,7 +24170,7 @@
       <c r="I17" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J17" s="21" t="b">
+      <c r="J17" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K17" s="21" t="s">
@@ -24211,7 +24209,7 @@
       <c r="I18" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J18" s="21" t="b">
+      <c r="J18" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K18" s="21" t="s">
@@ -24250,7 +24248,7 @@
       <c r="I19" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J19" s="21" t="b">
+      <c r="J19" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K19" s="21" t="s">
@@ -24289,7 +24287,7 @@
       <c r="I20" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J20" s="21" t="b">
+      <c r="J20" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K20" s="21" t="s">
@@ -24328,7 +24326,7 @@
       <c r="I21" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J21" s="21" t="b">
+      <c r="J21" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K21" s="21" t="s">
@@ -24367,7 +24365,7 @@
       <c r="I22" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J22" s="21" t="b">
+      <c r="J22" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K22" s="21" t="s">
@@ -24406,7 +24404,7 @@
       <c r="I23" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J23" s="21" t="b">
+      <c r="J23" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K23" s="21" t="s">
@@ -24445,7 +24443,7 @@
       <c r="I24" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J24" s="21" t="b">
+      <c r="J24" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K24" s="21" t="s">
@@ -24484,7 +24482,7 @@
       <c r="I25" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J25" s="21" t="b">
+      <c r="J25" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K25" s="21" t="s">
@@ -24523,7 +24521,7 @@
       <c r="I26" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J26" s="21" t="b">
+      <c r="J26" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K26" s="21" t="s">
@@ -24562,7 +24560,7 @@
       <c r="I27" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J27" s="21" t="b">
+      <c r="J27" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K27" s="21" t="s">
@@ -24601,7 +24599,7 @@
       <c r="I28" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J28" s="21" t="b">
+      <c r="J28" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K28" s="21" t="s">
@@ -24640,7 +24638,7 @@
       <c r="I29" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J29" s="21" t="b">
+      <c r="J29" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K29" s="21" t="s">
@@ -24679,7 +24677,7 @@
       <c r="I30" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J30" s="21" t="b">
+      <c r="J30" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K30" s="21" t="s">
@@ -24718,7 +24716,7 @@
       <c r="I31" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J31" s="21" t="b">
+      <c r="J31" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K31" s="21" t="s">
@@ -24757,7 +24755,7 @@
       <c r="I32" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J32" s="21" t="b">
+      <c r="J32" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K32" s="21" t="s">
@@ -24796,7 +24794,7 @@
       <c r="I33" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J33" s="21" t="b">
+      <c r="J33" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K33" s="21" t="s">
@@ -24835,7 +24833,7 @@
       <c r="I34" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J34" s="21" t="b">
+      <c r="J34" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K34" s="21" t="s">
@@ -24874,7 +24872,7 @@
       <c r="I35" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J35" s="21" t="b">
+      <c r="J35" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K35" s="21" t="s">
@@ -24913,7 +24911,7 @@
       <c r="I36" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J36" s="21" t="b">
+      <c r="J36" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K36" s="21" t="s">
@@ -24952,7 +24950,7 @@
       <c r="I37" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J37" s="21" t="b">
+      <c r="J37" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K37" s="21" t="s">
@@ -24991,7 +24989,7 @@
       <c r="I38" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J38" s="21" t="b">
+      <c r="J38" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K38" s="21" t="s">
@@ -25030,7 +25028,7 @@
       <c r="I39" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J39" s="21" t="b">
+      <c r="J39" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K39" s="21" t="s">
@@ -25069,7 +25067,7 @@
       <c r="I40" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J40" s="21" t="b">
+      <c r="J40" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K40" s="21" t="s">
@@ -25108,7 +25106,7 @@
       <c r="I41" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="J41" s="21" t="b">
+      <c r="J41" s="129" t="b">
         <v>0</v>
       </c>
       <c r="K41" s="21" t="s">

</xml_diff>